<commit_message>
MAINT: Part 1 v1.02
- Making changes after talk with instructor
</commit_message>
<xml_diff>
--- a/capstone/analysis_results/capstone.model_results.dataFrame.xlsx
+++ b/capstone/analysis_results/capstone.model_results.dataFrame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,18 +487,18 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.7556438127090301</v>
+        <v>0.8790450678460586</v>
       </c>
       <c r="E2" t="n">
-        <v>1.348732794324557</v>
+        <v>1.194809832175573</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>92.69921879200001</v>
+        <v>29.43540979200043</v>
       </c>
     </row>
     <row r="3">
@@ -518,18 +518,18 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.7557831661092531</v>
+        <v>0.8850742805651962</v>
       </c>
       <c r="E3" t="n">
-        <v>1.18960501352946</v>
+        <v>1.063429055611292</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>80.45878970800004</v>
+        <v>25.61203320801724</v>
       </c>
     </row>
     <row r="4">
@@ -549,18 +549,18 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.7557831661092531</v>
+        <v>0.8853213582527837</v>
       </c>
       <c r="E4" t="n">
-        <v>1.182779909173648</v>
+        <v>1.042586943507194</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>80.108657709</v>
+        <v>25.30355300000519</v>
       </c>
     </row>
     <row r="5">
@@ -580,18 +580,18 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.7550167224080268</v>
+        <v>0.8843010577267678</v>
       </c>
       <c r="E5" t="n">
-        <v>1.188147843877474</v>
+        <v>1.053470232089361</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>80.23260829099991</v>
+        <v>25.30541295898729</v>
       </c>
     </row>
     <row r="6">
@@ -611,18 +611,18 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.7603818283166109</v>
+        <v>0.8803191231606777</v>
       </c>
       <c r="E6" t="n">
-        <v>2.608903094132741</v>
+        <v>2.2069451212883</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "gini", "model__max_depth": 50, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>170.182083917</v>
+        <v>52.07366291698418</v>
       </c>
     </row>
     <row r="7">
@@ -642,18 +642,18 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.7653288740245262</v>
+        <v>0.8773545921411838</v>
       </c>
       <c r="E7" t="n">
-        <v>2.227073351542155</v>
+        <v>1.921985923250516</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "gini", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>145.2537764999997</v>
+        <v>43.79587774997344</v>
       </c>
     </row>
     <row r="8">
@@ -673,18 +673,18 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.7649108138238573</v>
+        <v>0.881237611588592</v>
       </c>
       <c r="E8" t="n">
-        <v>2.233899933099746</v>
+        <v>1.896561488509178</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>145.8017159999999</v>
+        <v>43.73308395899949</v>
       </c>
     </row>
     <row r="9">
@@ -704,18 +704,18 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.7594760312151616</v>
+        <v>0.8793293084365271</v>
       </c>
       <c r="E9" t="n">
-        <v>2.248465998967489</v>
+        <v>1.913800913095474</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "gini", "model__max_depth": 50, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>146.368992875</v>
+        <v>44.66518791698036</v>
       </c>
     </row>
     <row r="10">
@@ -735,18 +735,18 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7073578595317725</v>
+        <v>0.9315343353566843</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3190477561950684</v>
+        <v>0.3222541785240173</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>295.9302876670004</v>
+        <v>108.4233240419999</v>
       </c>
     </row>
     <row r="11">
@@ -766,18 +766,18 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.731953734671126</v>
+        <v>0.9427981581985472</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2703281998634338</v>
+        <v>0.2639323234558105</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": 500}</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>355.7119347920002</v>
+        <v>108.7184105830092</v>
       </c>
     </row>
     <row r="12">
@@ -797,18 +797,18 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.7270763656633222</v>
+        <v>0.9384841483577351</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2772646200656891</v>
+        <v>0.2704619228839874</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": 500}</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>277.1961012500005</v>
+        <v>98.60888470901409</v>
       </c>
     </row>
     <row r="13">
@@ -828,18 +828,18 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.7326505016722408</v>
+        <v>0.942642805890441</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2679497766494751</v>
+        <v>0.264656150341034</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": 500}</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>282.3464612079997</v>
+        <v>106.8641216249962</v>
       </c>
     </row>
     <row r="14">
@@ -859,18 +859,18 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.7908305462653289</v>
+        <v>0.9734723514605288</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3759302818775177</v>
+        <v>0.3164676284790039</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>440.4813412909998</v>
+        <v>115.3960450410086</v>
       </c>
     </row>
     <row r="15">
@@ -890,18 +890,18 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.784211259754738</v>
+        <v>0.9717685256335735</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3003611636161804</v>
+        <v>0.2610507738590241</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>390.7670815419997</v>
+        <v>152.728228833992</v>
       </c>
     </row>
     <row r="16">
@@ -921,18 +921,18 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.7866499442586399</v>
+        <v>0.9722435836478109</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3028792428970337</v>
+        <v>0.2696874761581421</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>365.6031451670005</v>
+        <v>99.70551920798607</v>
       </c>
     </row>
     <row r="17">
@@ -952,18 +952,18 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.784350613154961</v>
+        <v>0.9717381267377752</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2857414650917053</v>
+        <v>0.2474466335773468</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>323.2307480829995</v>
+        <v>180.872806667001</v>
       </c>
     </row>
     <row r="18">
@@ -983,10 +983,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.7673494983277592</v>
+        <v>0.9531746718651161</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3648868838946025</v>
+        <v>0.3027505179246266</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>15.0433293749993</v>
+        <v>5.602990082988981</v>
       </c>
     </row>
     <row r="19">
@@ -1014,10 +1014,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.7632385730211817</v>
+        <v>0.9543602927827028</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3083001375198364</v>
+        <v>0.2463798642158508</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>13.65727591599989</v>
+        <v>4.624882959004026</v>
       </c>
     </row>
     <row r="20">
@@ -1045,10 +1045,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.7699972129319955</v>
+        <v>0.95530242414735</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3259008109569549</v>
+        <v>0.263014413913091</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1056,7 +1056,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>13.63432283299971</v>
+        <v>4.775328999996418</v>
       </c>
     </row>
     <row r="21">
@@ -1076,10 +1076,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.7638656633221851</v>
+        <v>0.9544235529143363</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2974230806032817</v>
+        <v>0.2541276852289835</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>12.19615991699993</v>
+        <v>4.769068292021984</v>
       </c>
     </row>
     <row r="22">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.7722965440356745</v>
+        <v>0.964878063786201</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3744512875874837</v>
+        <v>0.3220246076583862</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>15.36693229200046</v>
+        <v>5.823270374996355</v>
       </c>
     </row>
     <row r="23">
@@ -1138,10 +1138,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.7694397993311036</v>
+        <v>0.9658474053973609</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3114554723103841</v>
+        <v>0.2522116561730703</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>12.72694362499988</v>
+        <v>4.76124137500301</v>
       </c>
     </row>
     <row r="24">
@@ -1169,10 +1169,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.7729933110367893</v>
+        <v>0.9659135341704523</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3111783663431804</v>
+        <v>0.2672414561112722</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>12.73094300000048</v>
+        <v>4.812960500014015</v>
       </c>
     </row>
     <row r="25">
@@ -1200,10 +1200,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.7694397993311036</v>
+        <v>0.9658473435737553</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2981161018212636</v>
+        <v>0.2468320687611898</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>12.21665037499952</v>
+        <v>4.627067333000014</v>
       </c>
     </row>
     <row r="26">
@@ -1231,10 +1231,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.7845596432552955</v>
+        <v>0.9443289950350515</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3466399053732554</v>
+        <v>0.2972681760787964</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>14.13765387500007</v>
+        <v>5.396360624989029</v>
       </c>
     </row>
     <row r="27">
@@ -1262,10 +1262,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.7773829431438127</v>
+        <v>0.9438206588065693</v>
       </c>
       <c r="E27" t="n">
-        <v>0.3368917504946391</v>
+        <v>0.2405405720074971</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>13.69854337499964</v>
+        <v>4.727558332990156</v>
       </c>
     </row>
     <row r="28">
@@ -1293,10 +1293,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.7810061315496098</v>
+        <v>0.9450599365446275</v>
       </c>
       <c r="E28" t="n">
-        <v>0.3236804266770681</v>
+        <v>0.2550284465154012</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1304,7 +1304,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>13.42499779199989</v>
+        <v>4.606934583018301</v>
       </c>
     </row>
     <row r="29">
@@ -1324,10 +1324,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.7765468227424749</v>
+        <v>0.943771473528919</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3499503930409749</v>
+        <v>0.2375452121098836</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>14.2841986250005</v>
+        <v>4.499347666016547</v>
       </c>
     </row>
     <row r="30">
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.7897853957636566</v>
+        <v>0.9710043812036906</v>
       </c>
       <c r="E30" t="n">
-        <v>0.404248317082723</v>
+        <v>0.2907109657923381</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1366,7 +1366,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>16.72838470900024</v>
+        <v>5.487691458984045</v>
       </c>
     </row>
     <row r="31">
@@ -1386,10 +1386,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.7791248606465998</v>
+        <v>0.9695185773428346</v>
       </c>
       <c r="E31" t="n">
-        <v>0.3505476852258047</v>
+        <v>0.2408114314079285</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>14.40786129099979</v>
+        <v>4.567891834012698</v>
       </c>
     </row>
     <row r="32">
@@ -1417,10 +1417,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.7873467112597548</v>
+        <v>0.9698537754072606</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3191726108392079</v>
+        <v>0.2529229283332825</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>13.07310799999959</v>
+        <v>4.638796374987578</v>
       </c>
     </row>
     <row r="33">
@@ -1448,10 +1448,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.7791248606465998</v>
+        <v>0.9695783102497578</v>
       </c>
       <c r="E33" t="n">
-        <v>0.3141185700893402</v>
+        <v>0.2392579515775045</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1459,7 +1459,7 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>12.94884483299938</v>
+        <v>4.524278208002215</v>
       </c>
     </row>
     <row r="34">
@@ -1479,18 +1479,18 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.7869983277591973</v>
+        <v>0.9586923088015173</v>
       </c>
       <c r="E34" t="n">
-        <v>121.7549864761034</v>
+        <v>90.3775022061666</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>{"model__C": 10, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 100, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>18838.972721917</v>
+        <v>6068.104392333014</v>
       </c>
     </row>
     <row r="35">
@@ -1510,18 +1510,18 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.7892279821627648</v>
+        <v>0.9603691484500572</v>
       </c>
       <c r="E35" t="n">
-        <v>71.07397664745649</v>
+        <v>57.12458638548851</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>{"model__C": 10, "model__l1_ratio": 0.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 100, "model__l1_ratio": 0.5, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>10933.584776667</v>
+        <v>3712.599043833005</v>
       </c>
     </row>
     <row r="36">
@@ -1541,18 +1541,18 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.7887402452619844</v>
+        <v>0.960091783075103</v>
       </c>
       <c r="E36" t="n">
-        <v>97.95748274008433</v>
+        <v>131.6969273602963</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>{"model__C": 10, "model__l1_ratio": 0.5, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 100, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>16368.772252708</v>
+        <v>8059.46575695902</v>
       </c>
     </row>
     <row r="37">
@@ -1572,18 +1572,18 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.7892976588628763</v>
+        <v>0.9603303572661535</v>
       </c>
       <c r="E37" t="n">
-        <v>70.68030965328217</v>
+        <v>102.6273009749254</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>{"model__C": 100, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 10, "model__l1_ratio": 0.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>11806.473676916</v>
+        <v>5399.201219375012</v>
       </c>
     </row>
     <row r="38">
@@ -1603,18 +1603,18 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.8643394648829431</v>
+        <v>0.98661685115662</v>
       </c>
       <c r="E38" t="n">
-        <v>30.58349098086357</v>
+        <v>43.29253586689632</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.5, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>4798.800575875001</v>
+        <v>2345.625237542001</v>
       </c>
     </row>
     <row r="39">
@@ -1634,18 +1634,18 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.8458054626532887</v>
+        <v>0.9840139522250123</v>
       </c>
       <c r="E39" t="n">
-        <v>22.99187534650167</v>
+        <v>41.10230638742447</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>3579.840115084007</v>
+        <v>2198.86051054101</v>
       </c>
     </row>
     <row r="40">
@@ -1665,18 +1665,18 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.8490802675585284</v>
+        <v>0.9849189233537254</v>
       </c>
       <c r="E40" t="n">
-        <v>40.53614270528157</v>
+        <v>40.23901522358258</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>4464.918524291003</v>
+        <v>2193.55761495902</v>
       </c>
     </row>
     <row r="41">
@@ -1696,18 +1696,762 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.8460841694537347</v>
+        <v>0.9840052129425053</v>
       </c>
       <c r="E41" t="n">
-        <v>23.09985637744268</v>
+        <v>41.16085040569305</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>3597.431578750009</v>
+        <v>2205.567522249999</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9859588231696181</v>
+      </c>
+      <c r="E42" t="n">
+        <v>11.99565851887067</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>831.3635886249831</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9852839919522474</v>
+      </c>
+      <c r="E43" t="n">
+        <v>9.742909802993138</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>691.1724815829948</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.9855884858753617</v>
+      </c>
+      <c r="E44" t="n">
+        <v>13.37820769713985</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.7, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>918.1099537080154</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.9852970436879072</v>
+      </c>
+      <c r="E45" t="n">
+        <v>15.2180129961835</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>1037.484150625009</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.9869954725563985</v>
+      </c>
+      <c r="E46" t="n">
+        <v>103.6930783228742</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>6421.626396209002</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.9858477943893839</v>
+      </c>
+      <c r="E47" t="n">
+        <v>89.54037327832644</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>5565.953025166993</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.9861815384593564</v>
+      </c>
+      <c r="E48" t="n">
+        <v>92.15152019891474</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>5716.530819666979</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.985966737897561</v>
+      </c>
+      <c r="E49" t="n">
+        <v>90.5555822753244</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 1, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>5631.057041916996</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.9651625612612003</v>
+      </c>
+      <c r="E50" t="n">
+        <v>174.8117938488722</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>1432.970788000006</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.9664369568545241</v>
+      </c>
+      <c r="E51" t="n">
+        <v>148.7001423150301</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>1223.369071166991</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.9644894608897217</v>
+      </c>
+      <c r="E52" t="n">
+        <v>134.6676911622286</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>1120.67374758402</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.9643416456508651</v>
+      </c>
+      <c r="E53" t="n">
+        <v>133.2518619894981</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1115.898864250019</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.9700922613181199</v>
+      </c>
+      <c r="E54" t="n">
+        <v>258.0679601281881</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>2199.784869374998</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.9703556166200668</v>
+      </c>
+      <c r="E55" t="n">
+        <v>215.0148673534393</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>1835.195166624995</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.9712287824715189</v>
+      </c>
+      <c r="E56" t="n">
+        <v>217.4656108409166</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>1849.731134375004</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.9712702706756078</v>
+      </c>
+      <c r="E57" t="n">
+        <v>218.3413614034653</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>1857.983143707999</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.9755662679587731</v>
+      </c>
+      <c r="E58" t="n">
+        <v>7.26015535692374</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>714.9583407920145</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.9768099552844349</v>
+      </c>
+      <c r="E59" t="n">
+        <v>7.271614888807139</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>705.0865867089597</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.977316111633714</v>
+      </c>
+      <c r="E60" t="n">
+        <v>6.936464201907316</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>681.9510156660108</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.9769164263524029</v>
+      </c>
+      <c r="E61" t="n">
+        <v>7.077846206724644</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>691.1364472500281</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.9778217950826862</v>
+      </c>
+      <c r="E62" t="n">
+        <v>8.81932769815127</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>838.9564697500318</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.9790889258763575</v>
+      </c>
+      <c r="E63" t="n">
+        <v>8.393872867524623</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>799.8681586250314</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.9791279564943463</v>
+      </c>
+      <c r="E64" t="n">
+        <v>7.952092997978132</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>762.6157083750004</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.9784742064192116</v>
+      </c>
+      <c r="E65" t="n">
+        <v>8.286464368800322</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>794.4221222919878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAINT: Part 1 v1.02 (#6)
- Making changes after talk with instructor

---------
Co-authored-by: Lloyd Gomes <gomes_la@hotmail.com>
</commit_message>
<xml_diff>
--- a/capstone/analysis_results/capstone.model_results.dataFrame.xlsx
+++ b/capstone/analysis_results/capstone.model_results.dataFrame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,18 +487,18 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.7556438127090301</v>
+        <v>0.8790450678460586</v>
       </c>
       <c r="E2" t="n">
-        <v>1.348732794324557</v>
+        <v>1.194809832175573</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>92.69921879200001</v>
+        <v>29.43540979200043</v>
       </c>
     </row>
     <row r="3">
@@ -518,18 +518,18 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.7557831661092531</v>
+        <v>0.8850742805651962</v>
       </c>
       <c r="E3" t="n">
-        <v>1.18960501352946</v>
+        <v>1.063429055611292</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>80.45878970800004</v>
+        <v>25.61203320801724</v>
       </c>
     </row>
     <row r="4">
@@ -549,18 +549,18 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.7557831661092531</v>
+        <v>0.8853213582527837</v>
       </c>
       <c r="E4" t="n">
-        <v>1.182779909173648</v>
+        <v>1.042586943507194</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>80.108657709</v>
+        <v>25.30355300000519</v>
       </c>
     </row>
     <row r="5">
@@ -580,18 +580,18 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.7550167224080268</v>
+        <v>0.8843010577267678</v>
       </c>
       <c r="E5" t="n">
-        <v>1.188147843877474</v>
+        <v>1.053470232089361</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>80.23260829099991</v>
+        <v>25.30541295898729</v>
       </c>
     </row>
     <row r="6">
@@ -611,18 +611,18 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.7603818283166109</v>
+        <v>0.8803191231606777</v>
       </c>
       <c r="E6" t="n">
-        <v>2.608903094132741</v>
+        <v>2.2069451212883</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "gini", "model__max_depth": 50, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>170.182083917</v>
+        <v>52.07366291698418</v>
       </c>
     </row>
     <row r="7">
@@ -642,18 +642,18 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.7653288740245262</v>
+        <v>0.8773545921411838</v>
       </c>
       <c r="E7" t="n">
-        <v>2.227073351542155</v>
+        <v>1.921985923250516</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "gini", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>145.2537764999997</v>
+        <v>43.79587774997344</v>
       </c>
     </row>
     <row r="8">
@@ -673,18 +673,18 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.7649108138238573</v>
+        <v>0.881237611588592</v>
       </c>
       <c r="E8" t="n">
-        <v>2.233899933099746</v>
+        <v>1.896561488509178</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "entropy", "model__max_depth": 25, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>145.8017159999999</v>
+        <v>43.73308395899949</v>
       </c>
     </row>
     <row r="9">
@@ -704,18 +704,18 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.7594760312151616</v>
+        <v>0.8793293084365271</v>
       </c>
       <c r="E9" t="n">
-        <v>2.248465998967489</v>
+        <v>1.913800913095474</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>{"model__criterion": "gini", "model__max_depth": 100, "vectorizer__max_features": null}</t>
+          <t>{"model__criterion": "gini", "model__max_depth": 50, "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>146.368992875</v>
+        <v>44.66518791698036</v>
       </c>
     </row>
     <row r="10">
@@ -735,18 +735,18 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7073578595317725</v>
+        <v>0.9315343353566843</v>
       </c>
       <c r="E10" t="n">
-        <v>0.3190477561950684</v>
+        <v>0.3222541785240173</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>295.9302876670004</v>
+        <v>108.4233240419999</v>
       </c>
     </row>
     <row r="11">
@@ -766,18 +766,18 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.731953734671126</v>
+        <v>0.9427981581985472</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2703281998634338</v>
+        <v>0.2639323234558105</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": 500}</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>355.7119347920002</v>
+        <v>108.7184105830092</v>
       </c>
     </row>
     <row r="12">
@@ -797,18 +797,18 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.7270763656633222</v>
+        <v>0.9384841483577351</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2772646200656891</v>
+        <v>0.2704619228839874</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": 500}</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>277.1961012500005</v>
+        <v>98.60888470901409</v>
       </c>
     </row>
     <row r="13">
@@ -828,18 +828,18 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.7326505016722408</v>
+        <v>0.942642805890441</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2679497766494751</v>
+        <v>0.264656150341034</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 10, "model__weights": "distance", "vectorizer__max_features": 500}</t>
+          <t>{"model__n_neighbors": 100, "model__weights": "distance", "vectorizer__max_features": 500}</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>282.3464612079997</v>
+        <v>106.8641216249962</v>
       </c>
     </row>
     <row r="14">
@@ -859,18 +859,18 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.7908305462653289</v>
+        <v>0.9734723514605288</v>
       </c>
       <c r="E14" t="n">
-        <v>0.3759302818775177</v>
+        <v>0.3164676284790039</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>440.4813412909998</v>
+        <v>115.3960450410086</v>
       </c>
     </row>
     <row r="15">
@@ -890,18 +890,18 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>0.784211259754738</v>
+        <v>0.9717685256335735</v>
       </c>
       <c r="E15" t="n">
-        <v>0.3003611636161804</v>
+        <v>0.2610507738590241</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>390.7670815419997</v>
+        <v>152.728228833992</v>
       </c>
     </row>
     <row r="16">
@@ -921,18 +921,18 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.7866499442586399</v>
+        <v>0.9722435836478109</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3028792428970337</v>
+        <v>0.2696874761581421</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>365.6031451670005</v>
+        <v>99.70551920798607</v>
       </c>
     </row>
     <row r="17">
@@ -952,18 +952,18 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.784350613154961</v>
+        <v>0.9717381267377752</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2857414650917053</v>
+        <v>0.2474466335773468</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>{"model__n_neighbors": 250, "model__weights": "distance", "vectorizer__max_features": null}</t>
+          <t>{"model__n_neighbors": 500, "model__weights": "distance", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>323.2307480829995</v>
+        <v>180.872806667001</v>
       </c>
     </row>
     <row r="18">
@@ -983,10 +983,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.7673494983277592</v>
+        <v>0.9531746718651161</v>
       </c>
       <c r="E18" t="n">
-        <v>0.3648868838946025</v>
+        <v>0.3027505179246266</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>15.0433293749993</v>
+        <v>5.602990082988981</v>
       </c>
     </row>
     <row r="19">
@@ -1014,10 +1014,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.7632385730211817</v>
+        <v>0.9543602927827028</v>
       </c>
       <c r="E19" t="n">
-        <v>0.3083001375198364</v>
+        <v>0.2463798642158508</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>13.65727591599989</v>
+        <v>4.624882959004026</v>
       </c>
     </row>
     <row r="20">
@@ -1045,10 +1045,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.7699972129319955</v>
+        <v>0.95530242414735</v>
       </c>
       <c r="E20" t="n">
-        <v>0.3259008109569549</v>
+        <v>0.263014413913091</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1056,7 +1056,7 @@
         </is>
       </c>
       <c r="G20" t="n">
-        <v>13.63432283299971</v>
+        <v>4.775328999996418</v>
       </c>
     </row>
     <row r="21">
@@ -1076,10 +1076,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.7638656633221851</v>
+        <v>0.9544235529143363</v>
       </c>
       <c r="E21" t="n">
-        <v>0.2974230806032817</v>
+        <v>0.2541276852289835</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>12.19615991699993</v>
+        <v>4.769068292021984</v>
       </c>
     </row>
     <row r="22">
@@ -1107,10 +1107,10 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0.7722965440356745</v>
+        <v>0.964878063786201</v>
       </c>
       <c r="E22" t="n">
-        <v>0.3744512875874837</v>
+        <v>0.3220246076583862</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>15.36693229200046</v>
+        <v>5.823270374996355</v>
       </c>
     </row>
     <row r="23">
@@ -1138,10 +1138,10 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.7694397993311036</v>
+        <v>0.9658474053973609</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3114554723103841</v>
+        <v>0.2522116561730703</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>12.72694362499988</v>
+        <v>4.76124137500301</v>
       </c>
     </row>
     <row r="24">
@@ -1169,10 +1169,10 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.7729933110367893</v>
+        <v>0.9659135341704523</v>
       </c>
       <c r="E24" t="n">
-        <v>0.3111783663431804</v>
+        <v>0.2672414561112722</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>12.73094300000048</v>
+        <v>4.812960500014015</v>
       </c>
     </row>
     <row r="25">
@@ -1200,10 +1200,10 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.7694397993311036</v>
+        <v>0.9658473435737553</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2981161018212636</v>
+        <v>0.2468320687611898</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>12.21665037499952</v>
+        <v>4.627067333000014</v>
       </c>
     </row>
     <row r="26">
@@ -1231,10 +1231,10 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.7845596432552955</v>
+        <v>0.9443289950350515</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3466399053732554</v>
+        <v>0.2972681760787964</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>14.13765387500007</v>
+        <v>5.396360624989029</v>
       </c>
     </row>
     <row r="27">
@@ -1262,10 +1262,10 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.7773829431438127</v>
+        <v>0.9438206588065693</v>
       </c>
       <c r="E27" t="n">
-        <v>0.3368917504946391</v>
+        <v>0.2405405720074971</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>13.69854337499964</v>
+        <v>4.727558332990156</v>
       </c>
     </row>
     <row r="28">
@@ -1293,10 +1293,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.7810061315496098</v>
+        <v>0.9450599365446275</v>
       </c>
       <c r="E28" t="n">
-        <v>0.3236804266770681</v>
+        <v>0.2550284465154012</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1304,7 +1304,7 @@
         </is>
       </c>
       <c r="G28" t="n">
-        <v>13.42499779199989</v>
+        <v>4.606934583018301</v>
       </c>
     </row>
     <row r="29">
@@ -1324,10 +1324,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0.7765468227424749</v>
+        <v>0.943771473528919</v>
       </c>
       <c r="E29" t="n">
-        <v>0.3499503930409749</v>
+        <v>0.2375452121098836</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>14.2841986250005</v>
+        <v>4.499347666016547</v>
       </c>
     </row>
     <row r="30">
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>0.7897853957636566</v>
+        <v>0.9710043812036906</v>
       </c>
       <c r="E30" t="n">
-        <v>0.404248317082723</v>
+        <v>0.2907109657923381</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1366,7 +1366,7 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>16.72838470900024</v>
+        <v>5.487691458984045</v>
       </c>
     </row>
     <row r="31">
@@ -1386,10 +1386,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.7791248606465998</v>
+        <v>0.9695185773428346</v>
       </c>
       <c r="E31" t="n">
-        <v>0.3505476852258047</v>
+        <v>0.2408114314079285</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1397,7 +1397,7 @@
         </is>
       </c>
       <c r="G31" t="n">
-        <v>14.40786129099979</v>
+        <v>4.567891834012698</v>
       </c>
     </row>
     <row r="32">
@@ -1417,10 +1417,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.7873467112597548</v>
+        <v>0.9698537754072606</v>
       </c>
       <c r="E32" t="n">
-        <v>0.3191726108392079</v>
+        <v>0.2529229283332825</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1428,7 +1428,7 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>13.07310799999959</v>
+        <v>4.638796374987578</v>
       </c>
     </row>
     <row r="33">
@@ -1448,10 +1448,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.7791248606465998</v>
+        <v>0.9695783102497578</v>
       </c>
       <c r="E33" t="n">
-        <v>0.3141185700893402</v>
+        <v>0.2392579515775045</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1459,7 +1459,7 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>12.94884483299938</v>
+        <v>4.524278208002215</v>
       </c>
     </row>
     <row r="34">
@@ -1479,18 +1479,18 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.7869983277591973</v>
+        <v>0.9586923088015173</v>
       </c>
       <c r="E34" t="n">
-        <v>121.7549864761034</v>
+        <v>90.3775022061666</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>{"model__C": 10, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 100, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>18838.972721917</v>
+        <v>6068.104392333014</v>
       </c>
     </row>
     <row r="35">
@@ -1510,18 +1510,18 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.7892279821627648</v>
+        <v>0.9603691484500572</v>
       </c>
       <c r="E35" t="n">
-        <v>71.07397664745649</v>
+        <v>57.12458638548851</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>{"model__C": 10, "model__l1_ratio": 0.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 100, "model__l1_ratio": 0.5, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>10933.584776667</v>
+        <v>3712.599043833005</v>
       </c>
     </row>
     <row r="36">
@@ -1541,18 +1541,18 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0.7887402452619844</v>
+        <v>0.960091783075103</v>
       </c>
       <c r="E36" t="n">
-        <v>97.95748274008433</v>
+        <v>131.6969273602963</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>{"model__C": 10, "model__l1_ratio": 0.5, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 100, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>16368.772252708</v>
+        <v>8059.46575695902</v>
       </c>
     </row>
     <row r="37">
@@ -1572,18 +1572,18 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.7892976588628763</v>
+        <v>0.9603303572661535</v>
       </c>
       <c r="E37" t="n">
-        <v>70.68030965328217</v>
+        <v>102.6273009749254</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>{"model__C": 100, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 10, "model__l1_ratio": 0.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>11806.473676916</v>
+        <v>5399.201219375012</v>
       </c>
     </row>
     <row r="38">
@@ -1603,18 +1603,18 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.8643394648829431</v>
+        <v>0.98661685115662</v>
       </c>
       <c r="E38" t="n">
-        <v>30.58349098086357</v>
+        <v>43.29253586689632</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.5, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>4798.800575875001</v>
+        <v>2345.625237542001</v>
       </c>
     </row>
     <row r="39">
@@ -1634,18 +1634,18 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.8458054626532887</v>
+        <v>0.9840139522250123</v>
       </c>
       <c r="E39" t="n">
-        <v>22.99187534650167</v>
+        <v>41.10230638742447</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>3579.840115084007</v>
+        <v>2198.86051054101</v>
       </c>
     </row>
     <row r="40">
@@ -1665,18 +1665,18 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.8490802675585284</v>
+        <v>0.9849189233537254</v>
       </c>
       <c r="E40" t="n">
-        <v>40.53614270528157</v>
+        <v>40.23901522358258</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>4464.918524291003</v>
+        <v>2193.55761495902</v>
       </c>
     </row>
     <row r="41">
@@ -1696,18 +1696,762 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.8460841694537347</v>
+        <v>0.9840052129425053</v>
       </c>
       <c r="E41" t="n">
-        <v>23.09985637744268</v>
+        <v>41.16085040569305</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>{"model__C": 1, "model__l1_ratio": 1.0, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
+          <t>{"model__C": 1, "model__l1_ratio": 0.25, "model__penalty": "elasticnet", "model__solver": "saga", "vectorizer__max_features": null}</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>3597.431578750009</v>
+        <v>2205.567522249999</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9859588231696181</v>
+      </c>
+      <c r="E42" t="n">
+        <v>11.99565851887067</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>831.3635886249831</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9852839919522474</v>
+      </c>
+      <c r="E43" t="n">
+        <v>9.742909802993138</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>691.1724815829948</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>0.9855884858753617</v>
+      </c>
+      <c r="E44" t="n">
+        <v>13.37820769713985</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.7, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>918.1099537080154</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0.9852970436879072</v>
+      </c>
+      <c r="E45" t="n">
+        <v>15.2180129961835</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>1037.484150625009</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>0.9869954725563985</v>
+      </c>
+      <c r="E46" t="n">
+        <v>103.6930783228742</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>6421.626396209002</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>0.9858477943893839</v>
+      </c>
+      <c r="E47" t="n">
+        <v>89.54037327832644</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>5565.953025166993</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>0.9861815384593564</v>
+      </c>
+      <c r="E48" t="n">
+        <v>92.15152019891474</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 0.7, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>5716.530819666979</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>XGBClassifier</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>0.985966737897561</v>
+      </c>
+      <c r="E49" t="n">
+        <v>90.5555822753244</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>{"model__colsample_bytree": 0.5, "model__max_depth": 10, "model__subsample": 1, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>5631.057041916996</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>0.9651625612612003</v>
+      </c>
+      <c r="E50" t="n">
+        <v>174.8117938488722</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>1432.970788000006</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>0.9664369568545241</v>
+      </c>
+      <c r="E51" t="n">
+        <v>148.7001423150301</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>1223.369071166991</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>0.9644894608897217</v>
+      </c>
+      <c r="E52" t="n">
+        <v>134.6676911622286</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>1120.67374758402</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0.9643416456508651</v>
+      </c>
+      <c r="E53" t="n">
+        <v>133.2518619894981</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>1115.898864250019</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0.9700922613181199</v>
+      </c>
+      <c r="E54" t="n">
+        <v>258.0679601281881</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>2199.784869374998</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>0.9703556166200668</v>
+      </c>
+      <c r="E55" t="n">
+        <v>215.0148673534393</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>1835.195166624995</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>0.9712287824715189</v>
+      </c>
+      <c r="E56" t="n">
+        <v>217.4656108409166</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>1849.731134375004</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BaggingClassifier</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>0.9712702706756078</v>
+      </c>
+      <c r="E57" t="n">
+        <v>218.3413614034653</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>{"model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>1857.983143707999</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>0.9755662679587731</v>
+      </c>
+      <c r="E58" t="n">
+        <v>7.26015535692374</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>714.9583407920145</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0.9768099552844349</v>
+      </c>
+      <c r="E59" t="n">
+        <v>7.271614888807139</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>705.0865867089597</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0.977316111633714</v>
+      </c>
+      <c r="E60" t="n">
+        <v>6.936464201907316</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>681.9510156660108</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CountVectorizer</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0.9769164263524029</v>
+      </c>
+      <c r="E61" t="n">
+        <v>7.077846206724644</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>691.1364472500281</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Original</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0.9778217950826862</v>
+      </c>
+      <c r="E62" t="n">
+        <v>8.81932769815127</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>838.9564697500318</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Stemmed</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0.9790889258763575</v>
+      </c>
+      <c r="E63" t="n">
+        <v>8.393872867524623</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>799.8681586250314</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Lemmatized</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0.9791279564943463</v>
+      </c>
+      <c r="E64" t="n">
+        <v>7.952092997978132</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>762.6157083750004</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>TfidfVectorizer</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Stemmed and Lemmatized</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>0.9784742064192116</v>
+      </c>
+      <c r="E65" t="n">
+        <v>8.286464368800322</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>{"model__class_weight": "balanced_subsample", "model__max_depth": 100, "model__n_estimators": 100, "vectorizer__max_features": null}</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>794.4221222919878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>